<commit_message>
Last commits before presentation
</commit_message>
<xml_diff>
--- a/src/main/java/com/got/app/database/towns.xlsx
+++ b/src/main/java/com/got/app/database/towns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/Library/Mobile Documents/com~apple~CloudDocs/College/YearTwo/SemesterTwo/DSII/code/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/Library/Mobile Documents/com~apple~CloudDocs/College/YearTwo/SemesterTwo/DSII/code/app/src/main/java/com/got/app/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7740442-7BAE-3847-9C8C-F4A8213E6B37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4666234-A247-6145-BE31-B5B83A3CA8FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -577,8 +577,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D61" sqref="A23:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1463,8 +1463,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A50" sqref="A1:D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>